<commit_message>
Scrubbed data off of the Excel Sheet
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sa_1/GitHub/inventory_utilities_v2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sa_1/GitHub/Inventory-Utilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="39320" windowHeight="19440" tabRatio="713" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="39320" windowHeight="19440" tabRatio="713" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="8" r:id="rId1"/>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="86">
   <si>
     <t>Ignore</t>
   </si>
@@ -464,12 +464,6 @@
     <t>g12-laas-hub-gw1/Chassis 1/Module 1/Ethernet1-2</t>
   </si>
   <si>
-    <t>MRV-116</t>
-  </si>
-  <si>
-    <t>qualias-eqx-01.force10networks.com</t>
-  </si>
-  <si>
     <t>./temp.log</t>
   </si>
   <si>
@@ -482,7 +476,10 @@
     <t>Device Names:</t>
   </si>
   <si>
-    <t>MRV-112</t>
+    <t>Test_CMTS</t>
+  </si>
+  <si>
+    <t>localhost</t>
   </si>
 </sst>
 </file>
@@ -1192,14 +1189,14 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1552,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1576,7 +1573,7 @@
         <v>45</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1605,10 +1602,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1616,7 +1613,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1651,11 +1648,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
       <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
@@ -1816,15 +1813,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="85.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="6" t="s">
         <v>19</v>
       </c>
@@ -1964,11 +1961,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="49.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
       <c r="D1" s="9">
         <v>42815</v>
       </c>
@@ -2128,11 +2125,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="55.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
       <c r="D1" s="10" t="s">
         <v>19</v>
       </c>
@@ -2218,10 +2215,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A5:A7"/>
+  <dimension ref="A5:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2231,17 +2228,12 @@
   <sheetData>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Logging and Custom Attributes to Shells
Reviewed and added logging, along with a log level selection in the
Excel file.
Implemented the Custom Attribute to Shell functionality
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="101">
   <si>
     <t>Ignore</t>
   </si>
@@ -508,6 +508,24 @@
   <si>
     <t>password</t>
   </si>
+  <si>
+    <t>log level</t>
+  </si>
+  <si>
+    <t>CRITICAL</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>WARNING</t>
+  </si>
+  <si>
+    <t>INFO</t>
+  </si>
+  <si>
+    <t>DEBUG</t>
+  </si>
 </sst>
 </file>
 
@@ -922,7 +940,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1096,21 +1114,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
@@ -1138,6 +1141,36 @@
         <color auto="1"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -1194,7 +1227,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1216,8 +1249,7 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1228,14 +1260,16 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="48">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1578,7 +1612,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="345.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1589,68 +1623,84 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="36" style="11" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="11"/>
+    <col min="3" max="3" width="0" style="11" hidden="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="25" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>44</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>48</v>
       </c>
@@ -1658,7 +1708,18 @@
         <v>65</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="12"/>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
+      <formula1>$C:$C</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1690,11 +1751,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
       <c r="E1" s="6" t="s">
         <v>17</v>
       </c>
@@ -1852,15 +1913,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="85.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="6" t="s">
         <v>17</v>
       </c>
@@ -1983,7 +2044,7 @@
       <c r="F7" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="18" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2041,7 +2102,7 @@
       <c r="F9" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="18" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2077,72 +2138,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="49.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
       <c r="D1" s="8">
         <v>42815</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="M4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="O4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="21" t="s">
+      <c r="P4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="Q4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="21" t="s">
+      <c r="R4" s="20" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2153,52 +2214,52 @@
       <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="J5" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="22" t="s">
+      <c r="K5" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="L5" s="22" t="s">
+      <c r="L5" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="22" t="s">
+      <c r="M5" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="N5" s="22" t="s">
+      <c r="N5" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="O5" s="22" t="s">
+      <c r="O5" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="P5" s="22" t="s">
+      <c r="P5" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="Q5" s="22" t="s">
+      <c r="Q5" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="R5" s="22" t="s">
+      <c r="R5" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2256,11 +2317,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="55.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
       <c r="D1" s="9" t="s">
         <v>17</v>
       </c>
@@ -2388,16 +2449,16 @@
       <c r="C29"/>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B30" s="15"/>
+      <c r="B30" s="14"/>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B31" s="15"/>
+      <c r="B31" s="14"/>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B32" s="15"/>
+      <c r="B32" s="14"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B33" s="15"/>
+      <c r="B33" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Revert "Fixed Log Level"
This reverts commit 3245bdf377183231491ad3858f01d7eb29e7b080.
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4480" windowWidth="38400" windowHeight="19440" tabRatio="713" activeTab="1"/>
+    <workbookView xWindow="1220" yWindow="5660" windowWidth="38400" windowHeight="19440" tabRatio="713" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="8" r:id="rId1"/>
@@ -503,6 +503,12 @@
     <t>NYC_02/Port_01</t>
   </si>
   <si>
+    <t>localhost</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
     <t>log level</t>
   </si>
   <si>
@@ -524,13 +530,7 @@
     <t>y</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>Tag_ID</t>
-  </si>
-  <si>
-    <t>localhost</t>
+    <t>Tag</t>
   </si>
 </sst>
 </file>
@@ -1636,7 +1636,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1655,7 +1655,7 @@
         <v>47</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1663,10 +1663,10 @@
         <v>41</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1674,10 +1674,10 @@
         <v>42</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1685,10 +1685,10 @@
         <v>43</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1699,7 +1699,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1720,10 +1720,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1801,7 +1801,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
@@ -1815,7 +1815,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
@@ -1829,7 +1829,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
@@ -1865,7 +1865,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>20</v>
@@ -1876,7 +1876,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>24</v>
@@ -1887,7 +1887,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>15</v>
@@ -1898,7 +1898,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>25</v>
@@ -1912,7 +1912,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added instructions on the List Connects tab
Added instructions to the Inventory.xlsx ‘List connections’ tab.
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="5660" windowWidth="38400" windowHeight="19440" tabRatio="713" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1460" windowWidth="26840" windowHeight="25800" tabRatio="713" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="8" r:id="rId1"/>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="122">
   <si>
     <t>Ignore</t>
   </si>
@@ -491,18 +491,12 @@
     <t>Kali</t>
   </si>
   <si>
-    <t>NYC_01/Port_01</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
     <t>Row 14 Rack 6</t>
   </si>
   <si>
-    <t>NYC_02/Port_01</t>
-  </si>
-  <si>
     <t>localhost</t>
   </si>
   <si>
@@ -531,6 +525,71 @@
   </si>
   <si>
     <t>Tag</t>
+  </si>
+  <si>
+    <t>Test_CMTS_1/port_1</t>
+  </si>
+  <si>
+    <t>Test_CMTS_1/port_10</t>
+  </si>
+  <si>
+    <t>Test_CMTS_1/port_11</t>
+  </si>
+  <si>
+    <t>Test_CMTS_1/port_12</t>
+  </si>
+  <si>
+    <t>Test_CMTS_1/port_13</t>
+  </si>
+  <si>
+    <t>Test_CMTS_1/port_14</t>
+  </si>
+  <si>
+    <t>Test_CMTS_1/port_15</t>
+  </si>
+  <si>
+    <t>Test_CMTS_1/port_16</t>
+  </si>
+  <si>
+    <t>Test_CMTS_1/port_17</t>
+  </si>
+  <si>
+    <t>Test_CMTS_1/port_18</t>
+  </si>
+  <si>
+    <t>Test_CMTS_2/port_1</t>
+  </si>
+  <si>
+    <t>Test_CMTS_2/port_10</t>
+  </si>
+  <si>
+    <t>Test_CMTS_2/port_11</t>
+  </si>
+  <si>
+    <t>Test_CMTS_2/port_12</t>
+  </si>
+  <si>
+    <t>Test_CMTS_2/port_13</t>
+  </si>
+  <si>
+    <t>Test_CMTS_2/port_14</t>
+  </si>
+  <si>
+    <t>Test_CMTS_2/port_15</t>
+  </si>
+  <si>
+    <t>Test_CMTS_2/port_16</t>
+  </si>
+  <si>
+    <t>Test_CMTS_2/port_17</t>
+  </si>
+  <si>
+    <t>Test_CMTS_2/port_18</t>
+  </si>
+  <si>
+    <t>Instructions:
+Enter the name of each device that you would like a listing of Children (cards &amp; ports) with a list of it's current connection, if any.  Will output to the same folder: "current_connections.csv"
+You can use this list to populate the '3-SetConnections' tab.</t>
   </si>
 </sst>
 </file>
@@ -753,7 +812,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -945,8 +1004,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1182,6 +1253,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1235,7 +1386,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1278,6 +1429,34 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1612,7 +1791,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="157" zoomScaleNormal="157" zoomScalePageLayoutView="157" workbookViewId="0">
+    <sheetView zoomScale="157" zoomScaleNormal="157" zoomScalePageLayoutView="157" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1635,9 +1814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="217" zoomScaleNormal="217" zoomScalePageLayoutView="217" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1655,7 +1832,7 @@
         <v>47</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1663,10 +1840,10 @@
         <v>41</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1677,7 +1854,7 @@
         <v>76</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1685,10 +1862,10 @@
         <v>43</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1699,7 +1876,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1720,10 +1897,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1744,7 +1921,7 @@
   </sheetPr>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="168" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1801,7 +1978,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
@@ -1815,7 +1992,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
@@ -1829,7 +2006,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -1843,7 +2020,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
@@ -1854,7 +2031,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
@@ -1865,7 +2042,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>20</v>
@@ -1876,7 +2053,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>24</v>
@@ -1887,7 +2064,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>15</v>
@@ -1898,7 +2075,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>25</v>
@@ -1912,7 +2089,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1932,8 +2109,8 @@
   </sheetPr>
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScale="173" zoomScaleNormal="173" zoomScalePageLayoutView="173" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2034,7 +2211,7 @@
         <v>11</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.15">
@@ -2075,7 +2252,7 @@
         <v>49</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.15">
@@ -2133,7 +2310,7 @@
         <v>49</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.15">
@@ -2170,8 +2347,8 @@
   </sheetPr>
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="173" zoomScaleNormal="173" zoomScalePageLayoutView="173" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2349,8 +2526,8 @@
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="250" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2397,47 +2574,83 @@
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7"/>
-      <c r="C7"/>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B8"/>
-      <c r="C8"/>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9"/>
-      <c r="C9"/>
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10"/>
-      <c r="C10"/>
+      <c r="B10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11"/>
-      <c r="C11"/>
+      <c r="B11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B12"/>
-      <c r="C12"/>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13"/>
-      <c r="C13"/>
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14"/>
-      <c r="C14"/>
+      <c r="B14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15"/>
-      <c r="C15"/>
+      <c r="B15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B16"/>
@@ -2522,10 +2735,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A5:A7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2533,22 +2746,59 @@
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="31"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="31"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="34"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Added User Report & Inventory Report
Added two new functions:
User Report - dumps a list of current users and some information
Inventory Report - Basic list of all top level items and non attribute
information (Domain, Reserved etc)
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -38,7 +38,7 @@
     <author>jibranna</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
     <author>jibranna</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -87,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0">
+    <comment ref="G5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -126,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0">
+    <comment ref="J5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +150,7 @@
     <author>jibranna</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -175,7 +175,7 @@
     <author>jibranna</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="123">
   <si>
     <t>Ignore</t>
   </si>
@@ -497,12 +497,6 @@
     <t>Row 14 Rack 6</t>
   </si>
   <si>
-    <t>localhost</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>log level</t>
   </si>
   <si>
@@ -590,12 +584,21 @@
     <t>Instructions:
 Enter the name of each device that you would like a listing of Children (cards &amp; ports) with a list of it's current connection, if any.  Will output to the same folder: "current_connections.csv"
 You can use this list to populate the '3-SetConnections' tab.</t>
+  </si>
+  <si>
+    <t>ksaper.homeip.net</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>808c$root</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1423,6 +1426,7 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1456,7 +1460,6 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1786,7 +1789,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1"/>
@@ -1814,7 +1817,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="217" zoomScaleNormal="217" zoomScalePageLayoutView="217" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="217" zoomScaleNormal="217" zoomScalePageLayoutView="217" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1832,7 +1837,7 @@
         <v>47</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1840,10 +1845,10 @@
         <v>41</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1851,10 +1856,10 @@
         <v>42</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1862,10 +1867,10 @@
         <v>43</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1876,7 +1881,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1897,10 +1902,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>93</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1916,7 +1921,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:F15"/>
@@ -1940,11 +1945,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
       <c r="E1" s="6" t="s">
         <v>17</v>
       </c>
@@ -1978,7 +1983,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
@@ -1992,7 +1997,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
@@ -2006,7 +2011,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -2020,7 +2025,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
@@ -2031,7 +2036,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
@@ -2042,7 +2047,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>20</v>
@@ -2053,7 +2058,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>24</v>
@@ -2064,7 +2069,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>15</v>
@@ -2075,7 +2080,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>25</v>
@@ -2089,7 +2094,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2104,7 +2109,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:R9"/>
@@ -2137,15 +2142,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="85.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
       <c r="H1" s="6" t="s">
         <v>17</v>
       </c>
@@ -2342,7 +2347,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:R7"/>
@@ -2362,11 +2367,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="49.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
       <c r="D1" s="8">
         <v>42815</v>
       </c>
@@ -2521,7 +2526,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:E33"/>
@@ -2541,11 +2546,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="55.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
       <c r="D1" s="9" t="s">
         <v>17</v>
       </c>
@@ -2574,82 +2579,82 @@
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
@@ -2732,7 +2737,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:F7"/>
@@ -2747,41 +2752,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28"/>
+      <c r="A1" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="32"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="34"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="24" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Update to Create and Autoload
For the main functionality - device creation - added in an Update
Option (attributes are already update), so this will allow address,
driver, location, domain updating (including removal from domain)
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1460" windowWidth="26840" windowHeight="25800" tabRatio="713" activeTab="1"/>
+    <workbookView xWindow="5340" yWindow="960" windowWidth="43000" windowHeight="26780" tabRatio="713" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="8" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="2-SetAttributes" sheetId="5" r:id="rId5"/>
     <sheet name="3-SetConnections" sheetId="6" r:id="rId6"/>
     <sheet name="4-ListConnections" sheetId="10" r:id="rId7"/>
+    <sheet name="5-UpdateUsers" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -33,12 +34,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>jibranna</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -67,12 +68,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>jibranna</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0" shapeId="0">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -87,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -102,13 +103,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -117,7 +118,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -126,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="K5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -145,12 +146,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>jibranna</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0" shapeId="0">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -170,23 +171,33 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>jibranna</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0" shapeId="0">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Y/N
-Row ignored if = Y</t>
+          <t xml:space="preserve">Y/N
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Row ignored if = Y</t>
         </r>
       </text>
     </comment>
@@ -195,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="148">
   <si>
     <t>Ignore</t>
   </si>
@@ -449,18 +460,12 @@
     <t>110.10.11.101</t>
   </si>
   <si>
-    <t>Servers</t>
-  </si>
-  <si>
     <t>root</t>
   </si>
   <si>
     <t>password1</t>
   </si>
   <si>
-    <t>enable</t>
-  </si>
-  <si>
     <t>Port_01</t>
   </si>
   <si>
@@ -468,9 +473,6 @@
   </si>
   <si>
     <t>GenericServer.ResourcePort</t>
-  </si>
-  <si>
-    <t>01</t>
   </si>
   <si>
     <t>NYC_02</t>
@@ -586,20 +588,106 @@
 You can use this list to populate the '3-SetConnections' tab.</t>
   </si>
   <si>
-    <t>ksaper.homeip.net</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>808c$root</t>
+    <t>Data Start on Row 5</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Is Active (Y/N)</t>
+  </si>
+  <si>
+    <t>Ignore (Y/N)</t>
+  </si>
+  <si>
+    <t>Add to Groups (Comma Separated)</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Remove from Groups (Comma Separated)</t>
+  </si>
+  <si>
+    <t>Science Group</t>
+  </si>
+  <si>
+    <t>Math Group</t>
+  </si>
+  <si>
+    <t>This Section is for updating User Information.  
+Username is the only Column Requried.  Use '*' to delete eMail</t>
+  </si>
+  <si>
+    <t>(Y/N)</t>
+  </si>
+  <si>
+    <t>Comma Separated</t>
+  </si>
+  <si>
+    <t>In Hours</t>
+  </si>
+  <si>
+    <t>Max Reservation Duration</t>
+  </si>
+  <si>
+    <t>Max Concurrent Reservations</t>
+  </si>
+  <si>
+    <t>"*" to delete</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Y/N</t>
+  </si>
+  <si>
+    <t>Only use if Subcomponent</t>
+  </si>
+  <si>
+    <t>ignored if updating</t>
+  </si>
+  <si>
+    <t>Eth-01</t>
+  </si>
+  <si>
+    <t>enable01</t>
+  </si>
+  <si>
+    <t>Servers/Dev</t>
+  </si>
+  <si>
+    <t>localhost</t>
+  </si>
+  <si>
+    <t>sysadmin</t>
+  </si>
+  <si>
+    <t>adminpassword</t>
+  </si>
+  <si>
+    <t>Comma Seperated
+add 'x_' to domain name to remove - *AMR,EMEA</t>
+  </si>
+  <si>
+    <t>AMR,x_Dev</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="29" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -813,6 +901,38 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="37">
@@ -1337,7 +1457,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1388,8 +1508,9 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1427,6 +1548,15 @@
     <xf numFmtId="0" fontId="25" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="50"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1460,8 +1590,11 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="15" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1503,6 +1636,7 @@
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1788,7 +1922,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -1798,12 +1932,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="143.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="345.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="345.5" customHeight="1">
       <c r="A1" s="16" t="s">
         <v>64</v>
       </c>
@@ -1814,14 +1948,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="217" zoomScaleNormal="217" zoomScalePageLayoutView="217" workbookViewId="0">
+    <sheetView zoomScale="217" zoomScaleNormal="217" zoomScalePageLayoutView="217" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="17.33203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="36" style="11" customWidth="1"/>
@@ -1829,7 +1963,7 @@
     <col min="4" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" thickBot="1">
       <c r="A1" s="22" t="s">
         <v>46</v>
       </c>
@@ -1837,43 +1971,43 @@
         <v>47</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="12" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="12" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="12" t="s">
         <v>44</v>
       </c>
@@ -1881,10 +2015,10 @@
         <v>45</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="12" t="s">
         <v>66</v>
       </c>
@@ -1892,7 +2026,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="12" t="s">
         <v>48</v>
       </c>
@@ -1900,17 +2034,17 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>91</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$C:$C</formula1>
     </dataValidation>
   </dataValidations>
@@ -1920,7 +2054,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -1930,7 +2064,7 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="7.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="37.6640625" style="1" customWidth="1"/>
@@ -1944,12 +2078,12 @@
     <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="73.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:6" ht="73.25" customHeight="1">
+      <c r="A1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
       <c r="E1" s="6" t="s">
         <v>17</v>
       </c>
@@ -1957,17 +2091,17 @@
         <v>42814</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="14">
       <c r="F3" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="13" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="13" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1981,9 +2115,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
@@ -1995,9 +2129,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
@@ -2009,9 +2143,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -2023,9 +2157,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
@@ -2034,9 +2168,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
@@ -2045,9 +2179,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>20</v>
@@ -2056,9 +2190,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>24</v>
@@ -2067,9 +2201,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>15</v>
@@ -2078,9 +2212,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>25</v>
@@ -2089,12 +2223,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6">
       <c r="B15" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2108,236 +2242,282 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView zoomScale="173" zoomScaleNormal="173" zoomScalePageLayoutView="173" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="173" zoomScalePageLayoutView="173" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="2" width="6.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="85.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:19" ht="85.25" customHeight="1">
+      <c r="A1" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="6" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="8">
+      <c r="J1" s="8">
         <v>42814</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="3" spans="1:19">
+      <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" s="29" customFormat="1" ht="37" thickBot="1">
+      <c r="A4" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="13" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="R5" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S5" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="B6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="N6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="B7" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="B8" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="H8" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="R6" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="C7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="S8" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="B9" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="B8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="C9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>82</v>
+      <c r="I9" s="18" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2346,17 +2526,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView zoomScale="173" zoomScaleNormal="173" zoomScalePageLayoutView="173" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.1640625" style="1" bestFit="1" customWidth="1"/>
@@ -2366,23 +2546,23 @@
     <col min="19" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="49.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:18" ht="49.25" customHeight="1">
+      <c r="A1" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="8">
         <v>42815</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18">
       <c r="D2" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="13" thickBot="1"/>
+    <row r="4" spans="1:18" ht="13" thickBot="1">
       <c r="A4" s="19" t="s">
         <v>18</v>
       </c>
@@ -2436,7 +2616,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="13" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2444,10 +2624,10 @@
         <v>27</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>50</v>
@@ -2492,23 +2672,23 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18">
       <c r="B6" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D6" s="1">
         <v>10.15</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18">
       <c r="B7" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D7" s="1">
         <v>2017.1</v>
@@ -2525,17 +2705,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="250" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C15"/>
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="40.1640625" style="1" customWidth="1"/>
@@ -2545,12 +2725,12 @@
     <col min="6" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="55.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:5" ht="55.25" customHeight="1">
+      <c r="A1" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
       <c r="D1" s="9" t="s">
         <v>17</v>
       </c>
@@ -2558,7 +2738,7 @@
         <v>42815</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -2566,7 +2746,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="13" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2577,152 +2757,152 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15">
       <c r="B6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15">
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15">
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15">
+      <c r="B9" t="s">
         <v>99</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+    <row r="10" spans="1:5" ht="15">
+      <c r="B10" t="s">
         <v>100</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C10" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+    <row r="11" spans="1:5" ht="15">
+      <c r="B11" t="s">
         <v>101</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+    <row r="12" spans="1:5" ht="15">
+      <c r="B12" t="s">
         <v>102</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="13" spans="1:5" ht="15">
+      <c r="B13" t="s">
         <v>103</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+    <row r="14" spans="1:5" ht="15">
+      <c r="B14" t="s">
         <v>104</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C14" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+    <row r="15" spans="1:5" ht="15">
+      <c r="B15" t="s">
         <v>105</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C15" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>107</v>
-      </c>
-      <c r="C14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>108</v>
-      </c>
-      <c r="C15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15">
       <c r="B16"/>
       <c r="C16"/>
     </row>
-    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" ht="15">
       <c r="B17"/>
       <c r="C17"/>
     </row>
-    <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" ht="15">
       <c r="B18"/>
       <c r="C18"/>
     </row>
-    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" ht="15">
       <c r="B19"/>
       <c r="C19"/>
     </row>
-    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" ht="15">
       <c r="B20"/>
       <c r="C20"/>
     </row>
-    <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" ht="15">
       <c r="B21"/>
       <c r="C21"/>
     </row>
-    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" ht="15">
       <c r="B22"/>
       <c r="C22"/>
     </row>
-    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" ht="15">
       <c r="B23"/>
       <c r="C23"/>
     </row>
-    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" ht="15">
       <c r="B24"/>
       <c r="C24"/>
     </row>
-    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" ht="15">
       <c r="B25"/>
       <c r="C25"/>
     </row>
-    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3" ht="15">
       <c r="B26"/>
       <c r="C26"/>
     </row>
-    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" ht="15">
       <c r="B27"/>
       <c r="C27"/>
     </row>
-    <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" ht="15">
       <c r="B28"/>
       <c r="C28"/>
     </row>
-    <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3" ht="15">
       <c r="B29"/>
       <c r="C29"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:3">
       <c r="B30" s="14"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:3">
       <c r="B31" s="14"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:3">
       <c r="B32" s="14"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:2">
       <c r="B33" s="14"/>
     </row>
   </sheetData>
@@ -2736,7 +2916,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
@@ -2746,56 +2926,56 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="29"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="32"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="33"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="35"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
+      <c r="A1" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="37"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="38"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="40"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="24" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -2807,4 +2987,125 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="300" zoomScaleNormal="300" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="3" width="20.83203125" customWidth="1"/>
+    <col min="5" max="6" width="33.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="26" customFormat="1" thickBot="1">
+      <c r="A4" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16" thickBot="1">
+      <c r="A5" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1" display="test@acmeco.com" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added Enable SNMP / Power Mgmt to Create&Autoload
Added two more columns to the Create_and_Autoload:
Enable SNMP - shell’s Enable SNMP for autoload (T/F)
Power Management - being power managed by CloudShell (T/F)
in addition updated the readme.md
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="960" windowWidth="43000" windowHeight="26780" tabRatio="713" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="23140" tabRatio="713" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="8" r:id="rId1"/>
@@ -79,12 +79,22 @@
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Y/N
-Row ignored if = Y</t>
+          <t xml:space="preserve">Y/N
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Row ignored if = Y</t>
         </r>
       </text>
     </comment>
@@ -206,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="151">
   <si>
     <t>Ignore</t>
   </si>
@@ -667,20 +677,29 @@
     <t>Servers/Dev</t>
   </si>
   <si>
+    <t>AMR,x_Dev</t>
+  </si>
+  <si>
     <t>localhost</t>
   </si>
   <si>
-    <t>sysadmin</t>
-  </si>
-  <si>
-    <t>adminpassword</t>
+    <t>adminuser</t>
+  </si>
+  <si>
+    <t>adminuserpassword</t>
+  </si>
+  <si>
+    <t>Y/N (default N)</t>
   </si>
   <si>
     <t>Comma Seperated
-add 'x_' to domain name to remove - *AMR,EMEA</t>
-  </si>
-  <si>
-    <t>AMR,x_Dev</t>
+add 'x_' to domain name to remove - x_AMR,EMEA</t>
+  </si>
+  <si>
+    <t>Enable SNMP</t>
+  </si>
+  <si>
+    <t>Under Power Mgmt</t>
   </si>
 </sst>
 </file>
@@ -1510,7 +1529,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1592,6 +1611,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1952,7 +1980,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="217" zoomScaleNormal="217" zoomScalePageLayoutView="217" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1979,7 +2007,7 @@
         <v>41</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>90</v>
@@ -1990,7 +2018,7 @@
         <v>42</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>91</v>
@@ -2001,7 +2029,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>92</v>
@@ -2246,18 +2274,16 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="173" zoomScalePageLayoutView="173" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="2" width="6.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" style="1" customWidth="1"/>
+    <col min="1" max="3" width="7.33203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="20.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="1" customWidth="1"/>
     <col min="7" max="7" width="26.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.83203125" style="1" customWidth="1"/>
@@ -2272,10 +2298,12 @@
     <col min="17" max="17" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.83203125" style="1"/>
+    <col min="20" max="20" width="8.83203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="12" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="85.25" customHeight="1">
+    <row r="1" spans="1:21" ht="85.25" customHeight="1">
       <c r="A1" s="30" t="s">
         <v>38</v>
       </c>
@@ -2293,12 +2321,12 @@
         <v>42814</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="29" customFormat="1" ht="37" thickBot="1">
+    <row r="4" spans="1:21" s="29" customFormat="1" ht="37" thickBot="1">
       <c r="A4" s="28" t="s">
         <v>137</v>
       </c>
@@ -2319,69 +2347,81 @@
         <v>139</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="13" thickBot="1">
-      <c r="A5" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="T4" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="U4" s="28" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="29" customFormat="1" ht="26" customHeight="1" thickBot="1">
+      <c r="A5" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="Q5" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="S5" s="43" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="T5" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="U5" s="44" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="B6" s="1" t="s">
         <v>124</v>
       </c>
@@ -2398,7 +2438,7 @@
         <v>73</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>74</v>
@@ -2428,7 +2468,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:21">
       <c r="B7" s="1" t="s">
         <v>124</v>
       </c>
@@ -2448,7 +2488,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:21">
       <c r="B8" s="1" t="s">
         <v>124</v>
       </c>
@@ -2465,7 +2505,7 @@
         <v>73</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>81</v>
@@ -2495,7 +2535,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:21">
       <c r="B9" s="1" t="s">
         <v>124</v>
       </c>
@@ -2712,7 +2752,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="250" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
@@ -2996,7 +3036,7 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="300" zoomScaleNormal="300" workbookViewId="0">
+    <sheetView zoomScale="300" zoomScaleNormal="300" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Bug fix on SNMP/Power Mgmt
Copy and paste fail, fixed reference to correct data field
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="23140" tabRatio="713" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="4180" windowWidth="51200" windowHeight="23140" tabRatio="713" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="8" r:id="rId1"/>
@@ -1529,7 +1529,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1563,13 +1563,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="50"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1621,6 +1618,13 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="50" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1992,10 +1996,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>47</v>
       </c>
       <c r="C1" s="11" t="s">
@@ -2107,11 +2111,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.25" customHeight="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
       <c r="E1" s="6" t="s">
         <v>17</v>
       </c>
@@ -2276,7 +2280,7 @@
   </sheetPr>
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="173" zoomScalePageLayoutView="173" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="173" zoomScaleNormal="173" zoomScalePageLayoutView="173" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -2304,16 +2308,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="85.25" customHeight="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="6" t="s">
         <v>17</v>
       </c>
@@ -2326,98 +2330,98 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="29" customFormat="1" ht="37" thickBot="1">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:21" s="26" customFormat="1" ht="37" thickBot="1">
+      <c r="A4" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28" t="s">
+      <c r="E4" s="25"/>
+      <c r="F4" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="T4" s="28" t="s">
+      <c r="T4" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="U4" s="28" t="s">
+      <c r="U4" s="25" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="29" customFormat="1" ht="26" customHeight="1" thickBot="1">
-      <c r="A5" s="42" t="s">
+    <row r="5" spans="1:21" s="26" customFormat="1" ht="26" customHeight="1" thickBot="1">
+      <c r="A5" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="43" t="s">
+      <c r="J5" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="43" t="s">
+      <c r="K5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="43" t="s">
+      <c r="L5" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="43" t="s">
+      <c r="M5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="43" t="s">
+      <c r="N5" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="43" t="s">
+      <c r="O5" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="43" t="s">
+      <c r="P5" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="43" t="s">
+      <c r="Q5" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="43" t="s">
+      <c r="R5" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="43" t="s">
+      <c r="S5" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="T5" s="43" t="s">
+      <c r="T5" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="U5" s="44" t="s">
+      <c r="U5" s="41" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2573,7 +2577,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView zoomScale="173" zoomScaleNormal="173" zoomScalePageLayoutView="173" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
@@ -2587,11 +2591,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="49.25" customHeight="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="8">
         <v>42815</v>
       </c>
@@ -2656,59 +2660,59 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="13" thickBot="1">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:18" s="26" customFormat="1" ht="24" customHeight="1" thickBot="1">
+      <c r="A5" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="K5" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="L5" s="21" t="s">
+      <c r="L5" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="21" t="s">
+      <c r="M5" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="N5" s="21" t="s">
+      <c r="N5" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="O5" s="21" t="s">
+      <c r="O5" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="P5" s="21" t="s">
+      <c r="P5" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="Q5" s="21" t="s">
+      <c r="Q5" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="R5" s="21" t="s">
+      <c r="R5" s="42" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2766,11 +2770,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="55.25" customHeight="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="9" t="s">
         <v>17</v>
       </c>
@@ -2962,7 +2966,7 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2972,41 +2976,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="35"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="37"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="37"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="38"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="40"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>68</v>
       </c>
     </row>
@@ -3036,53 +3040,54 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="300" zoomScaleNormal="300" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="2" max="3" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" style="43" customWidth="1"/>
     <col min="5" max="6" width="33.33203125" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="26" customFormat="1" thickBot="1">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:8" s="24" customFormat="1" thickBot="1">
+      <c r="A4" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="24" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3093,7 +3098,7 @@
       <c r="B5" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="45" t="s">
         <v>118</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -3119,7 +3124,7 @@
       <c r="B6" t="s">
         <v>123</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="46" t="s">
         <v>135</v>
       </c>
       <c r="D6" t="s">
@@ -3142,9 +3147,6 @@
   <mergeCells count="1">
     <mergeCell ref="A1:C2"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" display="test@acmeco.com" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>